<commit_message>
Build before Jenkins integration
Signed-off-by: mohit.kumar.bagadia <mohit.kumar.bagadia@HDC1-L-446FHJX.dir.svc.accenture.com>
</commit_message>
<xml_diff>
--- a/guru99/src/test/java/resources/testdata - Copy.xlsx
+++ b/guru99/src/test/java/resources/testdata - Copy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DEB2D7-E646-40B2-82A2-003BADCC367C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944FC2A5-78BA-4957-B3C0-0F6DB8E82242}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>usrname</t>
   </si>
@@ -77,34 +77,31 @@
     <t>TestState</t>
   </si>
   <si>
+    <t>cust ID</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>AccType</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>InitialDepositAmt</t>
+  </si>
+  <si>
+    <t>Account No</t>
+  </si>
+  <si>
     <t>f</t>
   </si>
   <si>
-    <t>cust ID</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>testacca1@gmail.com</t>
-  </si>
-  <si>
-    <t>testacca2@gmail.com</t>
-  </si>
-  <si>
-    <t>AccType</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>InitialDepositAmt</t>
-  </si>
-  <si>
-    <t>Account No</t>
+    <t>testacc3181@gmail.com</t>
+  </si>
+  <si>
+    <t>testacc3182@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -472,8 +469,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -508,21 +505,21 @@
         <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
         <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -543,19 +540,16 @@
         <v>123456</v>
       </c>
       <c r="H2">
-        <v>9999999999</v>
+        <v>1234567890</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J2">
         <v>123456</v>
       </c>
-      <c r="K2">
-        <v>42726</v>
-      </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -563,10 +557,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
         <v>11121989</v>
@@ -584,28 +578,25 @@
         <v>123456</v>
       </c>
       <c r="H3">
-        <v>9999999999</v>
+        <v>1234567890</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J3">
         <v>123456</v>
       </c>
-      <c r="K3">
-        <v>40270</v>
-      </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="M3">
-        <v>500</v>
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{6331ECF0-E070-4070-864C-B4B976FB9D81}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{631E4259-060D-48F1-A647-66F9E1FAD629}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{067757BC-B5FF-4EF2-AE54-E8F0A3714EAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>